<commit_message>
figure and script updates
</commit_message>
<xml_diff>
--- a/figures/paper/resistance_models.xlsx
+++ b/figures/paper/resistance_models.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git\arths-on-landscapes\figures\paper\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{198D0BDE-46DA-4595-8477-1D92EAC4BDEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEF41B73-AA0C-4834-A242-E782253D61DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,18 +27,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
-    <t>NLCD Land Cover Class</t>
-  </si>
-  <si>
-    <t>Model 1 Resistance Value</t>
-  </si>
-  <si>
-    <t>Model 2 Resistance Value</t>
-  </si>
-  <si>
-    <t>Model 3 Resistance Value</t>
-  </si>
-  <si>
     <t>Open Water</t>
   </si>
   <si>
@@ -57,9 +45,6 @@
     <t>Barren Land</t>
   </si>
   <si>
-    <t>Deciduous, Evergreen, or Mixed Forest</t>
-  </si>
-  <si>
     <t>Shrub/Scrub</t>
   </si>
   <si>
@@ -69,7 +54,22 @@
     <t>Pasture/Hay or Cultivated Crops</t>
   </si>
   <si>
-    <t>Woody Wetland or Emergent Herbaceous Wetland</t>
+    <t>Model 1</t>
+  </si>
+  <si>
+    <t>Model 2</t>
+  </si>
+  <si>
+    <t>Model 3</t>
+  </si>
+  <si>
+    <t>Land Cover Class</t>
+  </si>
+  <si>
+    <t>Wetlands</t>
+  </si>
+  <si>
+    <t>Forest</t>
   </si>
 </sst>
 </file>
@@ -115,18 +115,35 @@
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="6">
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -146,9 +163,6 @@
       </font>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -163,13 +177,18 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E7410C46-2E8E-4522-9104-6C1327AD6B8F}" name="Table1" displayName="Table1" ref="A1:D12" totalsRowShown="0" headerRowDxfId="0">
-  <autoFilter ref="A1:D12" xr:uid="{E7410C46-2E8E-4522-9104-6C1327AD6B8F}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E7410C46-2E8E-4522-9104-6C1327AD6B8F}" name="Table1" displayName="Table1" ref="B2:E13" totalsRowShown="0" headerRowDxfId="5" dataDxfId="0">
+  <autoFilter ref="B2:E13" xr:uid="{E7410C46-2E8E-4522-9104-6C1327AD6B8F}">
+    <filterColumn colId="0" hiddenButton="1"/>
+    <filterColumn colId="1" hiddenButton="1"/>
+    <filterColumn colId="2" hiddenButton="1"/>
+    <filterColumn colId="3" hiddenButton="1"/>
+  </autoFilter>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{246775E2-7E02-4FCE-9B2E-496D9BC10FDF}" name="NLCD Land Cover Class" dataDxfId="1"/>
-    <tableColumn id="2" xr3:uid="{8B6DECEC-02B8-47B5-A026-4E92829D2154}" name="Model 1 Resistance Value"/>
-    <tableColumn id="3" xr3:uid="{18FBE1AC-91D0-451E-B0AA-3F649DAB2811}" name="Model 2 Resistance Value"/>
-    <tableColumn id="4" xr3:uid="{626CE20D-81F2-417B-9E95-1CABC13B29D2}" name="Model 3 Resistance Value"/>
+    <tableColumn id="1" xr3:uid="{246775E2-7E02-4FCE-9B2E-496D9BC10FDF}" name="Land Cover Class" dataDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{8B6DECEC-02B8-47B5-A026-4E92829D2154}" name="Model 1" dataDxfId="3"/>
+    <tableColumn id="3" xr3:uid="{18FBE1AC-91D0-451E-B0AA-3F649DAB2811}" name="Model 2" dataDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{626CE20D-81F2-417B-9E95-1CABC13B29D2}" name="Model 3" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -438,185 +457,188 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D12"/>
+  <dimension ref="B1:E13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="29.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="22" style="3" customWidth="1"/>
-    <col min="2" max="2" width="16.6328125" customWidth="1"/>
-    <col min="3" max="3" width="15.453125" customWidth="1"/>
-    <col min="4" max="4" width="15.36328125" customWidth="1"/>
+    <col min="1" max="1" width="23.7265625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="18.90625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="9.7265625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="9.453125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="8.7265625" style="2" customWidth="1"/>
+    <col min="6" max="16384" width="29.81640625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="2:5" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="2:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B3" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C3" s="3">
+        <v>10</v>
+      </c>
+      <c r="D3" s="3">
+        <v>10</v>
+      </c>
+      <c r="E3" s="3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="B4" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C4" s="3">
+        <v>10</v>
+      </c>
+      <c r="D4" s="3">
+        <v>5</v>
+      </c>
+      <c r="E4" s="3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="B5" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="C5" s="3">
+        <v>10</v>
+      </c>
+      <c r="D5" s="3">
+        <v>10</v>
+      </c>
+      <c r="E5" s="3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B6" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="3">
+        <v>10</v>
+      </c>
+      <c r="D6" s="3">
+        <v>10</v>
+      </c>
+      <c r="E6" s="3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="B7" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A2" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2">
-        <v>10</v>
-      </c>
-      <c r="C2">
-        <v>10</v>
-      </c>
-      <c r="D2">
+      <c r="C7" s="3">
+        <v>10</v>
+      </c>
+      <c r="D7" s="3">
+        <v>10</v>
+      </c>
+      <c r="E7" s="3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B8" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="3">
+        <v>10</v>
+      </c>
+      <c r="D8" s="3">
+        <v>10</v>
+      </c>
+      <c r="E8" s="3">
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="3" t="s">
+    <row r="9" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B9" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" s="3">
+        <v>1</v>
+      </c>
+      <c r="D9" s="3">
+        <v>1</v>
+      </c>
+      <c r="E9" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B10" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" s="3">
+        <v>10</v>
+      </c>
+      <c r="D10" s="3">
         <v>5</v>
       </c>
-      <c r="B3">
-        <v>10</v>
-      </c>
-      <c r="C3">
+      <c r="E10" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B11" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11" s="3">
+        <v>10</v>
+      </c>
+      <c r="D11" s="3">
         <v>5</v>
       </c>
-      <c r="D3">
+      <c r="E11" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="2:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="B12" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C12" s="3">
+        <v>10</v>
+      </c>
+      <c r="D12" s="3">
+        <v>5</v>
+      </c>
+      <c r="E12" s="3">
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A4" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4">
-        <v>10</v>
-      </c>
-      <c r="C4">
-        <v>10</v>
-      </c>
-      <c r="D4">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="29" x14ac:dyDescent="0.35">
-      <c r="A5" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5">
-        <v>10</v>
-      </c>
-      <c r="C5">
-        <v>10</v>
-      </c>
-      <c r="D5">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6">
-        <v>10</v>
-      </c>
-      <c r="C6">
-        <v>10</v>
-      </c>
-      <c r="D6">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A7" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7">
-        <v>10</v>
-      </c>
-      <c r="C7">
-        <v>10</v>
-      </c>
-      <c r="D7">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="29" x14ac:dyDescent="0.35">
-      <c r="A8" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B8">
-        <v>1</v>
-      </c>
-      <c r="C8">
-        <v>1</v>
-      </c>
-      <c r="D8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A9" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B9">
-        <v>10</v>
-      </c>
-      <c r="C9">
+    <row r="13" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B13" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C13" s="3">
+        <v>10</v>
+      </c>
+      <c r="D13" s="3">
         <v>5</v>
       </c>
-      <c r="D9">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A10" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B10">
-        <v>10</v>
-      </c>
-      <c r="C10">
-        <v>5</v>
-      </c>
-      <c r="D10">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="29" x14ac:dyDescent="0.35">
-      <c r="A11" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B11">
-        <v>10</v>
-      </c>
-      <c r="C11">
-        <v>5</v>
-      </c>
-      <c r="D11">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A12" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B12">
-        <v>10</v>
-      </c>
-      <c r="C12">
-        <v>5</v>
-      </c>
-      <c r="D12">
+      <c r="E13" s="3">
         <v>1</v>
       </c>
     </row>

</xml_diff>